<commit_message>
Add basic layout for site
</commit_message>
<xml_diff>
--- a/simple.xlsx
+++ b/simple.xlsx
@@ -73,11 +73,11 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="18"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="9.68988764044944"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="6.389887640449439"/>
     <col min="2" max="2" bestFit="true" customWidth="true" width="8.589887640449438"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="15.18988764044944"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="11.88988764044944"/>
     <col min="4" max="4" bestFit="true" customWidth="true" width="15.18988764044944"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="12.989887640449439"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="15.18988764044944"/>
     <col min="6" max="6" bestFit="true" customWidth="true" width="7.489887640449439"/>
     <col min="7" max="7" bestFit="true" customWidth="true" width="25.08988764044944"/>
   </cols>
@@ -157,25 +157,25 @@
     <row r="3">
       <c r="A3" s="0" t="inlineStr">
         <is>
-          <t>Evangelina</t>
+          <t>andres</t>
         </is>
       </c>
       <c r="B3" s="0" t="inlineStr">
         <is>
-          <t>Tapia</t>
+          <t>perez</t>
         </is>
       </c>
       <c r="C3" s="0" t="inlineStr">
         <is>
-          <t>evangelina@chile.com</t>
+          <t>andres@chile.com</t>
         </is>
       </c>
       <c r="D3" s="0" t="n">
-        <v>81231212</v>
+        <v>51231212</v>
       </c>
       <c r="E3" s="0" t="inlineStr">
         <is>
-          <t>Los Frutillares 8993</t>
+          <t>Los conejitos 4321</t>
         </is>
       </c>
       <c r="F3" s="0" t="inlineStr">
@@ -185,7 +185,7 @@
       </c>
       <c r="G3" s="0" t="inlineStr">
         <is>
-          <t>29/05/2014 - 12:08:52</t>
+          <t>30/05/2014 - 16:21:57</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Add footer elements, dinamic position and color for slider label
</commit_message>
<xml_diff>
--- a/simple.xlsx
+++ b/simple.xlsx
@@ -67,17 +67,17 @@
   <sheetPr>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView windowProtection="false" tabSelected="false" showWhiteSpace="false" showOutlineSymbols="false" showFormulas="false" rightToLeft="false" showZeros="true" showRuler="true" showRowColHeaders="true" showGridLines="true" defaultGridColor="true" zoomScale="100" workbookViewId="0" zoomScaleSheetLayoutView="0" zoomScalePageLayoutView="0" zoomScaleNormal="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="18"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="6.389887640449439"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="12.989887640449439"/>
     <col min="2" max="2" bestFit="true" customWidth="true" width="8.589887640449438"/>
     <col min="3" max="3" bestFit="true" customWidth="true" width="11.88988764044944"/>
     <col min="4" max="4" bestFit="true" customWidth="true" width="15.18988764044944"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="15.18988764044944"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="26.18988764044944"/>
     <col min="6" max="6" bestFit="true" customWidth="true" width="7.489887640449439"/>
     <col min="7" max="7" bestFit="true" customWidth="true" width="25.08988764044944"/>
   </cols>
@@ -186,6 +186,33 @@
       <c r="G3" s="0" t="inlineStr">
         <is>
           <t>30/05/2014 - 16:21:57</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="0" t="inlineStr">
+        <is>
+          <t>Quam Ullamcorper</t>
+        </is>
+      </c>
+      <c r="B4" s="0"/>
+      <c r="C4" s="0" t="inlineStr">
+        <is>
+          <t>Justo@Lorem.com</t>
+        </is>
+      </c>
+      <c r="D4" s="0" t="n">
+        <v>61231212</v>
+      </c>
+      <c r="E4" s="0" t="inlineStr">
+        <is>
+          <t>Quam Adipiscing Parturient Justo 123</t>
+        </is>
+      </c>
+      <c r="F4" s="0"/>
+      <c r="G4" s="0" t="inlineStr">
+        <is>
+          <t>05/06/2014 - 18:25:52</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Add responsiveness for internal pages
</commit_message>
<xml_diff>
--- a/simple.xlsx
+++ b/simple.xlsx
@@ -67,7 +67,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView windowProtection="false" tabSelected="false" showWhiteSpace="false" showOutlineSymbols="false" showFormulas="false" rightToLeft="false" showZeros="true" showRuler="true" showRowColHeaders="true" showGridLines="true" defaultGridColor="true" zoomScale="100" workbookViewId="0" zoomScaleSheetLayoutView="0" zoomScalePageLayoutView="0" zoomScaleNormal="0"/>
   </sheetViews>
@@ -75,9 +75,9 @@
   <cols>
     <col min="1" max="1" bestFit="true" customWidth="true" width="11.88988764044944"/>
     <col min="2" max="2" bestFit="true" customWidth="true" width="8.589887640449438"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="9.68988764044944"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="12.989887640449439"/>
     <col min="4" max="4" bestFit="true" customWidth="true" width="15.18988764044944"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="19.58988764044944"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="21.789887640449443"/>
     <col min="6" max="6" bestFit="true" customWidth="true" width="5.289887640449439"/>
     <col min="7" max="7" bestFit="true" customWidth="true" width="25.08988764044944"/>
   </cols>
@@ -143,6 +143,149 @@
       <c r="G2" s="0" t="inlineStr">
         <is>
           <t>10/06/2014 - 14:47:54</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="0" t="inlineStr">
+        <is>
+          <t>asdasdasdasd</t>
+        </is>
+      </c>
+      <c r="B3" s="0"/>
+      <c r="C3" s="0" t="inlineStr">
+        <is>
+          <t>asdasd</t>
+        </is>
+      </c>
+      <c r="D3" s="0" t="inlineStr">
+        <is>
+          <t>asdasd</t>
+        </is>
+      </c>
+      <c r="E3" s="0" t="inlineStr">
+        <is>
+          <t>asdasd</t>
+        </is>
+      </c>
+      <c r="F3" s="0"/>
+      <c r="G3" s="0" t="inlineStr">
+        <is>
+          <t>12/06/2014 - 03:05:19</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="0" t="inlineStr">
+        <is>
+          <t>asdasd</t>
+        </is>
+      </c>
+      <c r="B4" s="0"/>
+      <c r="C4" s="0" t="inlineStr">
+        <is>
+          <t>asdasd</t>
+        </is>
+      </c>
+      <c r="D4" s="0" t="inlineStr">
+        <is>
+          <t>asdasd</t>
+        </is>
+      </c>
+      <c r="E4" s="0" t="inlineStr">
+        <is>
+          <t>asdasd</t>
+        </is>
+      </c>
+      <c r="F4" s="0"/>
+      <c r="G4" s="0" t="inlineStr">
+        <is>
+          <t>12/06/2014 - 03:05:59</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="0" t="inlineStr">
+        <is>
+          <t>asdasd</t>
+        </is>
+      </c>
+      <c r="B5" s="0"/>
+      <c r="C5" s="0" t="inlineStr">
+        <is>
+          <t>asdasd</t>
+        </is>
+      </c>
+      <c r="D5" s="0" t="inlineStr">
+        <is>
+          <t>asdasd</t>
+        </is>
+      </c>
+      <c r="E5" s="0" t="inlineStr">
+        <is>
+          <t>asdasda</t>
+        </is>
+      </c>
+      <c r="F5" s="0"/>
+      <c r="G5" s="0" t="inlineStr">
+        <is>
+          <t>12/06/2014 - 03:06:23</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="0" t="inlineStr">
+        <is>
+          <t>Josesito</t>
+        </is>
+      </c>
+      <c r="B6" s="0"/>
+      <c r="C6" s="0" t="inlineStr">
+        <is>
+          <t>Jiseselito@josnrn.hhsj</t>
+        </is>
+      </c>
+      <c r="D6" s="0" t="inlineStr">
+        <is>
+          <t>62727:73</t>
+        </is>
+      </c>
+      <c r="E6" s="0" t="inlineStr">
+        <is>
+          <t>Jesús jdjd k 123</t>
+        </is>
+      </c>
+      <c r="F6" s="0"/>
+      <c r="G6" s="0" t="inlineStr">
+        <is>
+          <t>13/06/2014 - 22:23:41</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="0" t="inlineStr">
+        <is>
+          <t>evangelina tapia</t>
+        </is>
+      </c>
+      <c r="B7" s="0"/>
+      <c r="C7" s="0" t="inlineStr">
+        <is>
+          <t>eva@chile.com</t>
+        </is>
+      </c>
+      <c r="D7" s="0" t="n">
+        <v>61231234</v>
+      </c>
+      <c r="E7" s="0" t="inlineStr">
+        <is>
+          <t>Los Conejitos Blanquitos 123</t>
+        </is>
+      </c>
+      <c r="F7" s="0"/>
+      <c r="G7" s="0" t="inlineStr">
+        <is>
+          <t>16/06/2014 - 21:19:54</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Fixes and implement feeback client
</commit_message>
<xml_diff>
--- a/simple.xlsx
+++ b/simple.xlsx
@@ -67,7 +67,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView windowProtection="false" tabSelected="false" showWhiteSpace="false" showOutlineSymbols="false" showFormulas="false" rightToLeft="false" showZeros="true" showRuler="true" showRowColHeaders="true" showGridLines="true" defaultGridColor="true" zoomScale="100" workbookViewId="0" zoomScaleSheetLayoutView="0" zoomScalePageLayoutView="0" zoomScaleNormal="0"/>
   </sheetViews>
@@ -149,7 +149,7 @@
     <row r="3">
       <c r="A3" s="0" t="inlineStr">
         <is>
-          <t>asdasdasdasd</t>
+          <t>asdasd</t>
         </is>
       </c>
       <c r="B3" s="0"/>
@@ -171,7 +171,7 @@
       <c r="F3" s="0"/>
       <c r="G3" s="0" t="inlineStr">
         <is>
-          <t>12/06/2014 - 03:05:19</t>
+          <t>12/06/2014 - 03:05:59</t>
         </is>
       </c>
     </row>
@@ -194,96 +194,67 @@
       </c>
       <c r="E4" s="0" t="inlineStr">
         <is>
-          <t>asdasd</t>
+          <t>asdasda</t>
         </is>
       </c>
       <c r="F4" s="0"/>
       <c r="G4" s="0" t="inlineStr">
         <is>
-          <t>12/06/2014 - 03:05:59</t>
+          <t>12/06/2014 - 03:06:23</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="0" t="inlineStr">
         <is>
-          <t>asdasd</t>
+          <t>Josesito</t>
         </is>
       </c>
       <c r="B5" s="0"/>
       <c r="C5" s="0" t="inlineStr">
         <is>
-          <t>asdasd</t>
+          <t>Jiseselito@josnrn.hhsj</t>
         </is>
       </c>
       <c r="D5" s="0" t="inlineStr">
         <is>
-          <t>asdasd</t>
+          <t>62727:73</t>
         </is>
       </c>
       <c r="E5" s="0" t="inlineStr">
         <is>
-          <t>asdasda</t>
+          <t>Jesús jdjd k 123</t>
         </is>
       </c>
       <c r="F5" s="0"/>
       <c r="G5" s="0" t="inlineStr">
         <is>
-          <t>12/06/2014 - 03:06:23</t>
+          <t>13/06/2014 - 22:23:41</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="0" t="inlineStr">
         <is>
-          <t>Josesito</t>
+          <t>evangelina tapia</t>
         </is>
       </c>
       <c r="B6" s="0"/>
       <c r="C6" s="0" t="inlineStr">
         <is>
-          <t>Jiseselito@josnrn.hhsj</t>
-        </is>
-      </c>
-      <c r="D6" s="0" t="inlineStr">
-        <is>
-          <t>62727:73</t>
-        </is>
+          <t>eva@chile.com</t>
+        </is>
+      </c>
+      <c r="D6" s="0" t="n">
+        <v>61231234</v>
       </c>
       <c r="E6" s="0" t="inlineStr">
         <is>
-          <t>Jesús jdjd k 123</t>
+          <t>Los Conejitos Blanquitos 123</t>
         </is>
       </c>
       <c r="F6" s="0"/>
       <c r="G6" s="0" t="inlineStr">
-        <is>
-          <t>13/06/2014 - 22:23:41</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="0" t="inlineStr">
-        <is>
-          <t>evangelina tapia</t>
-        </is>
-      </c>
-      <c r="B7" s="0"/>
-      <c r="C7" s="0" t="inlineStr">
-        <is>
-          <t>eva@chile.com</t>
-        </is>
-      </c>
-      <c r="D7" s="0" t="n">
-        <v>61231234</v>
-      </c>
-      <c r="E7" s="0" t="inlineStr">
-        <is>
-          <t>Los Conejitos Blanquitos 123</t>
-        </is>
-      </c>
-      <c r="F7" s="0"/>
-      <c r="G7" s="0" t="inlineStr">
         <is>
           <t>16/06/2014 - 21:19:54</t>
         </is>

</xml_diff>